<commit_message>
moved simulator files to folder
</commit_message>
<xml_diff>
--- a/Data/Final Project Data/energy usage.xlsx
+++ b/Data/Final Project Data/energy usage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rutvikdoshi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rutvikdoshi/dev/python/q-learn-final/ST-Yau-Physics/Data/Final Project Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B461B9-9D87-364D-B988-7D057D699A2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFE9B39-71E7-F749-A380-98953D5F41DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" xr2:uid="{44E61D18-BE46-8E49-808C-3CA49572E768}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Relay Controller</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Energy Supplied (1st 10 minutes)</t>
+  </si>
+  <si>
+    <t>Energy Supplied till 2nd oscillation</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -162,8 +165,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Compariative Energy Usage</a:t>
+              <a:rPr lang="en-GB" b="1"/>
+              <a:t>Comparing Energy Usage across all 4 controllers</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -181,7 +184,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -343,6 +346,77 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4DB-494C-921E-7F2EFC464BA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Energy Supplied till 2nd oscillation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Relay Controller</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>PID Controller</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Reinforcement Learning Model 1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Reinforcement Learning Model 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2779</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1861</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-94F1-2F41-91DB-3F570B856A8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1157,10 +1231,10 @@
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1485,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B9B410-1772-2D49-B4F8-D3A164DC74A6}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B4" sqref="B4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,6 +1621,23 @@
         <v>1854</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6160</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3916</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2779</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1861</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>